<commit_message>
SMT Part Class Total Quantity Calculation
</commit_message>
<xml_diff>
--- a/Resources/Total_Qty_Calculation.xlsx
+++ b/Resources/Total_Qty_Calculation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="204">
   <si>
     <t>Line Item</t>
   </si>
@@ -212,48 +212,6 @@
     <t>SMT CP</t>
   </si>
   <si>
-    <t>IND-THT DIP</t>
-  </si>
-  <si>
-    <t>IND-THT DISC</t>
-  </si>
-  <si>
-    <t>IND-THT EP</t>
-  </si>
-  <si>
-    <t>IND-THT TOROID</t>
-  </si>
-  <si>
-    <t>INSULATO ALL</t>
-  </si>
-  <si>
-    <t>LABEL ALL</t>
-  </si>
-  <si>
-    <t>LCD ALL</t>
-  </si>
-  <si>
-    <t>LED-SMT ALL</t>
-  </si>
-  <si>
-    <t>LED-THT ALL</t>
-  </si>
-  <si>
-    <t>METAL BOX</t>
-  </si>
-  <si>
-    <t>METAL CHASSIS</t>
-  </si>
-  <si>
-    <t>METAL COVER</t>
-  </si>
-  <si>
-    <t>METAL FRAME</t>
-  </si>
-  <si>
-    <t>METAL OTHER</t>
-  </si>
-  <si>
     <t>METAL SHIELD</t>
   </si>
   <si>
@@ -657,6 +615,18 @@
   </si>
   <si>
     <t>50.85</t>
+  </si>
+  <si>
+    <t>0.0001</t>
+  </si>
+  <si>
+    <t>5.85</t>
+  </si>
+  <si>
+    <t>C0402C562K3RACTU78</t>
+  </si>
+  <si>
+    <t>16SEPC100M91011</t>
   </si>
 </sst>
 </file>
@@ -1262,7 +1232,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1323,6 +1293,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="22" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -2292,7 +2267,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2300,29 +2275,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R234"/>
+  <dimension ref="A1:Q220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" style="6" customWidth="1"/>
     <col min="3" max="3" width="42.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125"/>
     <col min="5" max="5" width="17" style="6" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" style="2" customWidth="1"/>
-    <col min="7" max="8" width="14.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="26" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="6" customWidth="1"/>
     <col min="9" max="9" width="15" style="6" customWidth="1"/>
     <col min="10" max="10" width="19.85546875" style="2" customWidth="1"/>
     <col min="11" max="11" width="26" style="2" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125"/>
     <col min="14" max="14" width="15.140625" customWidth="1"/>
     <col min="15" max="15" width="18.140625" customWidth="1"/>
     <col min="16" max="16" width="24" style="1" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="26.28515625" style="2" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="19.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -2344,11 +2321,11 @@
       <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="27" t="s">
         <v>50</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>51</v>
@@ -2384,35 +2361,35 @@
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="20" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="F2" s="22"/>
       <c r="G2" s="25" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="H2" s="13">
         <v>1</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="K2" s="23" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
@@ -2429,35 +2406,35 @@
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="20" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="F3" s="22"/>
       <c r="G3" s="25" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="H3" s="13">
         <v>2</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -2474,35 +2451,35 @@
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="20" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="25" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="H4" s="13">
         <v>3</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="N4" s="13"/>
       <c r="O4" s="13"/>
@@ -2516,35 +2493,35 @@
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="20" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="25" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="H5" s="13">
         <v>4</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
@@ -2558,35 +2535,35 @@
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="20" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="25" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="H6" s="13">
         <v>5</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="N6" s="13"/>
       <c r="O6" s="13"/>
@@ -2600,35 +2577,35 @@
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="20" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="25" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="H7" s="13">
         <v>6</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
@@ -2637,19 +2614,41 @@
       </c>
     </row>
     <row r="8" spans="1:17" s="4" customFormat="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" s="22"/>
+      <c r="G8" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="H8" s="13">
+        <v>7</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>171</v>
+      </c>
       <c r="N8" s="13"/>
       <c r="O8" s="13"/>
       <c r="P8" s="4" t="s">
@@ -2657,19 +2656,41 @@
       </c>
     </row>
     <row r="9" spans="1:17" s="4" customFormat="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="F9" s="22"/>
+      <c r="G9" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="H9" s="13">
+        <v>8</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>171</v>
+      </c>
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
       <c r="P9" s="4" t="s">
@@ -2677,19 +2698,41 @@
       </c>
     </row>
     <row r="10" spans="1:17" s="4" customFormat="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="H10" s="13">
+        <v>9</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>171</v>
+      </c>
       <c r="N10" s="13"/>
       <c r="O10" s="13"/>
       <c r="P10" s="4" t="s">
@@ -2697,19 +2740,41 @@
       </c>
     </row>
     <row r="11" spans="1:17" s="4" customFormat="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="F11" s="22"/>
+      <c r="G11" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="H11" s="13">
+        <v>10</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>171</v>
+      </c>
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
       <c r="P11" s="4" t="s">
@@ -2717,19 +2782,41 @@
       </c>
     </row>
     <row r="12" spans="1:17" s="4" customFormat="1">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="F12" s="22"/>
+      <c r="G12" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="H12" s="13">
+        <v>11</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>171</v>
+      </c>
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
       <c r="P12" s="4" t="s">
@@ -2743,7 +2830,7 @@
       <c r="D13" s="7"/>
       <c r="E13" s="12"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="13"/>
+      <c r="G13" s="28"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
       <c r="J13" s="5"/>
@@ -2763,7 +2850,7 @@
       <c r="D14" s="7"/>
       <c r="E14" s="12"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="13"/>
+      <c r="G14" s="28"/>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
       <c r="J14" s="5"/>
@@ -2783,7 +2870,7 @@
       <c r="D15" s="7"/>
       <c r="E15" s="12"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="13"/>
+      <c r="G15" s="28"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
       <c r="J15" s="5"/>
@@ -2803,7 +2890,7 @@
       <c r="D16" s="7"/>
       <c r="E16" s="12"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="13"/>
+      <c r="G16" s="28"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
       <c r="J16" s="5"/>
@@ -2823,7 +2910,7 @@
       <c r="D17" s="7"/>
       <c r="E17" s="12"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="13"/>
+      <c r="G17" s="28"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
       <c r="J17" s="5"/>
@@ -2843,7 +2930,7 @@
       <c r="D18" s="7"/>
       <c r="E18" s="12"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="13"/>
+      <c r="G18" s="28"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
       <c r="J18" s="5"/>
@@ -2863,7 +2950,7 @@
       <c r="D19" s="7"/>
       <c r="E19" s="12"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="13"/>
+      <c r="G19" s="28"/>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
       <c r="J19" s="5"/>
@@ -2883,7 +2970,7 @@
       <c r="D20" s="7"/>
       <c r="E20" s="12"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="13"/>
+      <c r="G20" s="28"/>
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
       <c r="J20" s="5"/>
@@ -2903,7 +2990,7 @@
       <c r="D21" s="7"/>
       <c r="E21" s="12"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="13"/>
+      <c r="G21" s="28"/>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
       <c r="J21" s="5"/>
@@ -2923,7 +3010,7 @@
       <c r="D22" s="7"/>
       <c r="E22" s="12"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="13"/>
+      <c r="G22" s="28"/>
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
       <c r="J22" s="5"/>
@@ -2943,7 +3030,7 @@
       <c r="D23" s="7"/>
       <c r="E23" s="12"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="13"/>
+      <c r="G23" s="28"/>
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
       <c r="J23" s="5"/>
@@ -2963,7 +3050,7 @@
       <c r="D24" s="7"/>
       <c r="E24" s="12"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="13"/>
+      <c r="G24" s="28"/>
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
       <c r="J24" s="5"/>
@@ -2983,7 +3070,7 @@
       <c r="D25" s="7"/>
       <c r="E25" s="12"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="13"/>
+      <c r="G25" s="28"/>
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
       <c r="J25" s="5"/>
@@ -3003,7 +3090,7 @@
       <c r="D26" s="7"/>
       <c r="E26" s="12"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="13"/>
+      <c r="G26" s="28"/>
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
       <c r="J26" s="5"/>
@@ -3023,7 +3110,7 @@
       <c r="D27" s="7"/>
       <c r="E27" s="12"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="13"/>
+      <c r="G27" s="28"/>
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
       <c r="J27" s="5"/>
@@ -3043,7 +3130,7 @@
       <c r="D28" s="7"/>
       <c r="E28" s="12"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="13"/>
+      <c r="G28" s="28"/>
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
       <c r="J28" s="5"/>
@@ -3063,7 +3150,7 @@
       <c r="D29" s="7"/>
       <c r="E29" s="12"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="13"/>
+      <c r="G29" s="28"/>
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
       <c r="J29" s="5"/>
@@ -3083,7 +3170,7 @@
       <c r="D30" s="7"/>
       <c r="E30" s="12"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="13"/>
+      <c r="G30" s="28"/>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
       <c r="J30" s="5"/>
@@ -3103,7 +3190,7 @@
       <c r="D31" s="7"/>
       <c r="E31" s="12"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="13"/>
+      <c r="G31" s="28"/>
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
       <c r="J31" s="5"/>
@@ -3123,7 +3210,7 @@
       <c r="D32" s="7"/>
       <c r="E32" s="12"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="13"/>
+      <c r="G32" s="28"/>
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
       <c r="J32" s="5"/>
@@ -3143,7 +3230,7 @@
       <c r="D33" s="7"/>
       <c r="E33" s="12"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="13"/>
+      <c r="G33" s="28"/>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
       <c r="J33" s="5"/>
@@ -3163,7 +3250,7 @@
       <c r="D34" s="7"/>
       <c r="E34" s="12"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="13"/>
+      <c r="G34" s="28"/>
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
       <c r="J34" s="5"/>
@@ -3183,7 +3270,7 @@
       <c r="D35" s="7"/>
       <c r="E35" s="12"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="13"/>
+      <c r="G35" s="28"/>
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
       <c r="J35" s="5"/>
@@ -3203,7 +3290,7 @@
       <c r="D36" s="7"/>
       <c r="E36" s="12"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="13"/>
+      <c r="G36" s="28"/>
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
       <c r="J36" s="5"/>
@@ -3223,7 +3310,7 @@
       <c r="D37" s="7"/>
       <c r="E37" s="12"/>
       <c r="F37" s="5"/>
-      <c r="G37" s="13"/>
+      <c r="G37" s="28"/>
       <c r="H37" s="13"/>
       <c r="I37" s="13"/>
       <c r="J37" s="5"/>
@@ -3243,7 +3330,7 @@
       <c r="D38" s="7"/>
       <c r="E38" s="12"/>
       <c r="F38" s="5"/>
-      <c r="G38" s="13"/>
+      <c r="G38" s="28"/>
       <c r="H38" s="13"/>
       <c r="I38" s="13"/>
       <c r="J38" s="5"/>
@@ -3263,7 +3350,7 @@
       <c r="D39" s="7"/>
       <c r="E39" s="12"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="13"/>
+      <c r="G39" s="28"/>
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
       <c r="J39" s="5"/>
@@ -3283,7 +3370,7 @@
       <c r="D40" s="7"/>
       <c r="E40" s="12"/>
       <c r="F40" s="5"/>
-      <c r="G40" s="13"/>
+      <c r="G40" s="28"/>
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
       <c r="J40" s="5"/>
@@ -3303,7 +3390,7 @@
       <c r="D41" s="7"/>
       <c r="E41" s="12"/>
       <c r="F41" s="5"/>
-      <c r="G41" s="13"/>
+      <c r="G41" s="28"/>
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
       <c r="J41" s="5"/>
@@ -3323,7 +3410,7 @@
       <c r="D42" s="7"/>
       <c r="E42" s="12"/>
       <c r="F42" s="5"/>
-      <c r="G42" s="13"/>
+      <c r="G42" s="28"/>
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
       <c r="J42" s="5"/>
@@ -3343,7 +3430,7 @@
       <c r="D43" s="7"/>
       <c r="E43" s="12"/>
       <c r="F43" s="5"/>
-      <c r="G43" s="13"/>
+      <c r="G43" s="28"/>
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
       <c r="J43" s="5"/>
@@ -3363,7 +3450,7 @@
       <c r="D44" s="7"/>
       <c r="E44" s="12"/>
       <c r="F44" s="5"/>
-      <c r="G44" s="13"/>
+      <c r="G44" s="28"/>
       <c r="H44" s="13"/>
       <c r="I44" s="13"/>
       <c r="J44" s="5"/>
@@ -3383,7 +3470,7 @@
       <c r="D45" s="7"/>
       <c r="E45" s="12"/>
       <c r="F45" s="5"/>
-      <c r="G45" s="13"/>
+      <c r="G45" s="28"/>
       <c r="H45" s="13"/>
       <c r="I45" s="13"/>
       <c r="J45" s="5"/>
@@ -3403,7 +3490,7 @@
       <c r="D46" s="7"/>
       <c r="E46" s="12"/>
       <c r="F46" s="5"/>
-      <c r="G46" s="13"/>
+      <c r="G46" s="28"/>
       <c r="H46" s="13"/>
       <c r="I46" s="13"/>
       <c r="J46" s="5"/>
@@ -3423,7 +3510,7 @@
       <c r="D47" s="7"/>
       <c r="E47" s="12"/>
       <c r="F47" s="5"/>
-      <c r="G47" s="13"/>
+      <c r="G47" s="28"/>
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
       <c r="J47" s="5"/>
@@ -3443,7 +3530,7 @@
       <c r="D48" s="7"/>
       <c r="E48" s="12"/>
       <c r="F48" s="5"/>
-      <c r="G48" s="13"/>
+      <c r="G48" s="28"/>
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
       <c r="J48" s="5"/>
@@ -3463,7 +3550,7 @@
       <c r="D49" s="7"/>
       <c r="E49" s="12"/>
       <c r="F49" s="5"/>
-      <c r="G49" s="13"/>
+      <c r="G49" s="28"/>
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
       <c r="J49" s="5"/>
@@ -3483,7 +3570,7 @@
       <c r="D50" s="7"/>
       <c r="E50" s="12"/>
       <c r="F50" s="5"/>
-      <c r="G50" s="13"/>
+      <c r="G50" s="28"/>
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
       <c r="J50" s="5"/>
@@ -3503,7 +3590,7 @@
       <c r="D51" s="7"/>
       <c r="E51" s="12"/>
       <c r="F51" s="5"/>
-      <c r="G51" s="13"/>
+      <c r="G51" s="28"/>
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>
       <c r="J51" s="5"/>
@@ -3523,7 +3610,7 @@
       <c r="D52" s="7"/>
       <c r="E52" s="12"/>
       <c r="F52" s="5"/>
-      <c r="G52" s="13"/>
+      <c r="G52" s="28"/>
       <c r="H52" s="13"/>
       <c r="I52" s="13"/>
       <c r="J52" s="5"/>
@@ -3543,7 +3630,7 @@
       <c r="D53" s="7"/>
       <c r="E53" s="12"/>
       <c r="F53" s="5"/>
-      <c r="G53" s="13"/>
+      <c r="G53" s="28"/>
       <c r="H53" s="13"/>
       <c r="I53" s="13"/>
       <c r="J53" s="5"/>
@@ -3563,7 +3650,7 @@
       <c r="D54" s="7"/>
       <c r="E54" s="12"/>
       <c r="F54" s="5"/>
-      <c r="G54" s="13"/>
+      <c r="G54" s="28"/>
       <c r="H54" s="13"/>
       <c r="I54" s="13"/>
       <c r="J54" s="5"/>
@@ -3583,7 +3670,7 @@
       <c r="D55" s="7"/>
       <c r="E55" s="12"/>
       <c r="F55" s="5"/>
-      <c r="G55" s="13"/>
+      <c r="G55" s="28"/>
       <c r="H55" s="13"/>
       <c r="I55" s="13"/>
       <c r="J55" s="5"/>
@@ -3603,7 +3690,7 @@
       <c r="D56" s="7"/>
       <c r="E56" s="12"/>
       <c r="F56" s="5"/>
-      <c r="G56" s="13"/>
+      <c r="G56" s="28"/>
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
       <c r="J56" s="5"/>
@@ -3623,7 +3710,7 @@
       <c r="D57" s="7"/>
       <c r="E57" s="12"/>
       <c r="F57" s="5"/>
-      <c r="G57" s="13"/>
+      <c r="G57" s="28"/>
       <c r="H57" s="13"/>
       <c r="I57" s="13"/>
       <c r="J57" s="5"/>
@@ -3643,7 +3730,7 @@
       <c r="D58" s="7"/>
       <c r="E58" s="12"/>
       <c r="F58" s="5"/>
-      <c r="G58" s="13"/>
+      <c r="G58" s="28"/>
       <c r="H58" s="13"/>
       <c r="I58" s="13"/>
       <c r="J58" s="5"/>
@@ -3663,7 +3750,7 @@
       <c r="D59" s="7"/>
       <c r="E59" s="12"/>
       <c r="F59" s="5"/>
-      <c r="G59" s="13"/>
+      <c r="G59" s="28"/>
       <c r="H59" s="13"/>
       <c r="I59" s="13"/>
       <c r="J59" s="5"/>
@@ -3683,7 +3770,7 @@
       <c r="D60" s="7"/>
       <c r="E60" s="12"/>
       <c r="F60" s="5"/>
-      <c r="G60" s="13"/>
+      <c r="G60" s="28"/>
       <c r="H60" s="13"/>
       <c r="I60" s="13"/>
       <c r="J60" s="5"/>
@@ -3703,7 +3790,7 @@
       <c r="D61" s="7"/>
       <c r="E61" s="12"/>
       <c r="F61" s="5"/>
-      <c r="G61" s="13"/>
+      <c r="G61" s="28"/>
       <c r="H61" s="13"/>
       <c r="I61" s="13"/>
       <c r="J61" s="5"/>
@@ -3723,7 +3810,7 @@
       <c r="D62" s="7"/>
       <c r="E62" s="12"/>
       <c r="F62" s="5"/>
-      <c r="G62" s="13"/>
+      <c r="G62" s="28"/>
       <c r="H62" s="13"/>
       <c r="I62" s="13"/>
       <c r="J62" s="5"/>
@@ -3743,7 +3830,7 @@
       <c r="D63" s="7"/>
       <c r="E63" s="12"/>
       <c r="F63" s="5"/>
-      <c r="G63" s="13"/>
+      <c r="G63" s="28"/>
       <c r="H63" s="13"/>
       <c r="I63" s="13"/>
       <c r="J63" s="5"/>
@@ -3763,7 +3850,7 @@
       <c r="D64" s="7"/>
       <c r="E64" s="12"/>
       <c r="F64" s="5"/>
-      <c r="G64" s="13"/>
+      <c r="G64" s="28"/>
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
       <c r="J64" s="5"/>
@@ -3783,7 +3870,7 @@
       <c r="D65" s="7"/>
       <c r="E65" s="12"/>
       <c r="F65" s="5"/>
-      <c r="G65" s="13"/>
+      <c r="G65" s="28"/>
       <c r="H65" s="13"/>
       <c r="I65" s="13"/>
       <c r="J65" s="5"/>
@@ -3803,7 +3890,7 @@
       <c r="D66" s="7"/>
       <c r="E66" s="12"/>
       <c r="F66" s="5"/>
-      <c r="G66" s="13"/>
+      <c r="G66" s="28"/>
       <c r="H66" s="13"/>
       <c r="I66" s="13"/>
       <c r="J66" s="5"/>
@@ -3823,7 +3910,7 @@
       <c r="D67" s="7"/>
       <c r="E67" s="12"/>
       <c r="F67" s="5"/>
-      <c r="G67" s="13"/>
+      <c r="G67" s="28"/>
       <c r="H67" s="13"/>
       <c r="I67" s="13"/>
       <c r="J67" s="5"/>
@@ -3843,7 +3930,7 @@
       <c r="D68" s="7"/>
       <c r="E68" s="12"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="13"/>
+      <c r="G68" s="28"/>
       <c r="H68" s="13"/>
       <c r="I68" s="13"/>
       <c r="J68" s="5"/>
@@ -3863,7 +3950,7 @@
       <c r="D69" s="7"/>
       <c r="E69" s="12"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="13"/>
+      <c r="G69" s="28"/>
       <c r="H69" s="13"/>
       <c r="I69" s="13"/>
       <c r="J69" s="5"/>
@@ -3883,7 +3970,7 @@
       <c r="D70" s="7"/>
       <c r="E70" s="12"/>
       <c r="F70" s="5"/>
-      <c r="G70" s="13"/>
+      <c r="G70" s="28"/>
       <c r="H70" s="13"/>
       <c r="I70" s="13"/>
       <c r="J70" s="5"/>
@@ -3903,7 +3990,7 @@
       <c r="D71" s="7"/>
       <c r="E71" s="12"/>
       <c r="F71" s="5"/>
-      <c r="G71" s="13"/>
+      <c r="G71" s="28"/>
       <c r="H71" s="13"/>
       <c r="I71" s="13"/>
       <c r="J71" s="5"/>
@@ -3923,7 +4010,7 @@
       <c r="D72" s="7"/>
       <c r="E72" s="12"/>
       <c r="F72" s="5"/>
-      <c r="G72" s="13"/>
+      <c r="G72" s="28"/>
       <c r="H72" s="13"/>
       <c r="I72" s="13"/>
       <c r="J72" s="5"/>
@@ -3943,7 +4030,7 @@
       <c r="D73" s="7"/>
       <c r="E73" s="12"/>
       <c r="F73" s="5"/>
-      <c r="G73" s="13"/>
+      <c r="G73" s="28"/>
       <c r="H73" s="13"/>
       <c r="I73" s="13"/>
       <c r="J73" s="5"/>
@@ -3963,7 +4050,7 @@
       <c r="D74" s="7"/>
       <c r="E74" s="12"/>
       <c r="F74" s="5"/>
-      <c r="G74" s="13"/>
+      <c r="G74" s="28"/>
       <c r="H74" s="13"/>
       <c r="I74" s="13"/>
       <c r="J74" s="5"/>
@@ -3983,7 +4070,7 @@
       <c r="D75" s="7"/>
       <c r="E75" s="12"/>
       <c r="F75" s="5"/>
-      <c r="G75" s="13"/>
+      <c r="G75" s="28"/>
       <c r="H75" s="13"/>
       <c r="I75" s="13"/>
       <c r="J75" s="5"/>
@@ -4003,7 +4090,7 @@
       <c r="D76" s="7"/>
       <c r="E76" s="12"/>
       <c r="F76" s="5"/>
-      <c r="G76" s="13"/>
+      <c r="G76" s="28"/>
       <c r="H76" s="13"/>
       <c r="I76" s="13"/>
       <c r="J76" s="5"/>
@@ -4023,7 +4110,7 @@
       <c r="D77" s="7"/>
       <c r="E77" s="12"/>
       <c r="F77" s="5"/>
-      <c r="G77" s="13"/>
+      <c r="G77" s="28"/>
       <c r="H77" s="13"/>
       <c r="I77" s="13"/>
       <c r="J77" s="5"/>
@@ -4043,7 +4130,7 @@
       <c r="D78" s="7"/>
       <c r="E78" s="12"/>
       <c r="F78" s="5"/>
-      <c r="G78" s="13"/>
+      <c r="G78" s="28"/>
       <c r="H78" s="13"/>
       <c r="I78" s="13"/>
       <c r="J78" s="5"/>
@@ -4063,7 +4150,7 @@
       <c r="D79" s="7"/>
       <c r="E79" s="12"/>
       <c r="F79" s="5"/>
-      <c r="G79" s="13"/>
+      <c r="G79" s="28"/>
       <c r="H79" s="13"/>
       <c r="I79" s="13"/>
       <c r="J79" s="5"/>
@@ -4083,7 +4170,7 @@
       <c r="D80" s="7"/>
       <c r="E80" s="12"/>
       <c r="F80" s="5"/>
-      <c r="G80" s="13"/>
+      <c r="G80" s="28"/>
       <c r="H80" s="13"/>
       <c r="I80" s="13"/>
       <c r="J80" s="5"/>
@@ -4103,7 +4190,7 @@
       <c r="D81" s="7"/>
       <c r="E81" s="12"/>
       <c r="F81" s="5"/>
-      <c r="G81" s="13"/>
+      <c r="G81" s="28"/>
       <c r="H81" s="13"/>
       <c r="I81" s="13"/>
       <c r="J81" s="5"/>
@@ -4123,7 +4210,7 @@
       <c r="D82" s="7"/>
       <c r="E82" s="12"/>
       <c r="F82" s="5"/>
-      <c r="G82" s="13"/>
+      <c r="G82" s="28"/>
       <c r="H82" s="13"/>
       <c r="I82" s="13"/>
       <c r="J82" s="5"/>
@@ -4143,7 +4230,7 @@
       <c r="D83" s="7"/>
       <c r="E83" s="12"/>
       <c r="F83" s="5"/>
-      <c r="G83" s="13"/>
+      <c r="G83" s="28"/>
       <c r="H83" s="13"/>
       <c r="I83" s="13"/>
       <c r="J83" s="5"/>
@@ -4163,7 +4250,7 @@
       <c r="D84" s="7"/>
       <c r="E84" s="12"/>
       <c r="F84" s="5"/>
-      <c r="G84" s="13"/>
+      <c r="G84" s="28"/>
       <c r="H84" s="13"/>
       <c r="I84" s="13"/>
       <c r="J84" s="5"/>
@@ -4183,7 +4270,7 @@
       <c r="D85" s="7"/>
       <c r="E85" s="12"/>
       <c r="F85" s="5"/>
-      <c r="G85" s="13"/>
+      <c r="G85" s="28"/>
       <c r="H85" s="13"/>
       <c r="I85" s="13"/>
       <c r="J85" s="5"/>
@@ -4203,7 +4290,7 @@
       <c r="D86" s="7"/>
       <c r="E86" s="12"/>
       <c r="F86" s="5"/>
-      <c r="G86" s="13"/>
+      <c r="G86" s="28"/>
       <c r="H86" s="13"/>
       <c r="I86" s="13"/>
       <c r="J86" s="5"/>
@@ -4223,7 +4310,7 @@
       <c r="D87" s="7"/>
       <c r="E87" s="12"/>
       <c r="F87" s="5"/>
-      <c r="G87" s="13"/>
+      <c r="G87" s="28"/>
       <c r="H87" s="13"/>
       <c r="I87" s="13"/>
       <c r="J87" s="5"/>
@@ -4243,7 +4330,7 @@
       <c r="D88" s="7"/>
       <c r="E88" s="12"/>
       <c r="F88" s="5"/>
-      <c r="G88" s="13"/>
+      <c r="G88" s="28"/>
       <c r="H88" s="13"/>
       <c r="I88" s="13"/>
       <c r="J88" s="5"/>
@@ -4263,7 +4350,7 @@
       <c r="D89" s="7"/>
       <c r="E89" s="12"/>
       <c r="F89" s="5"/>
-      <c r="G89" s="13"/>
+      <c r="G89" s="28"/>
       <c r="H89" s="13"/>
       <c r="I89" s="13"/>
       <c r="J89" s="5"/>
@@ -4283,7 +4370,7 @@
       <c r="D90" s="7"/>
       <c r="E90" s="12"/>
       <c r="F90" s="5"/>
-      <c r="G90" s="13"/>
+      <c r="G90" s="28"/>
       <c r="H90" s="13"/>
       <c r="I90" s="13"/>
       <c r="J90" s="5"/>
@@ -4303,7 +4390,7 @@
       <c r="D91" s="7"/>
       <c r="E91" s="12"/>
       <c r="F91" s="5"/>
-      <c r="G91" s="13"/>
+      <c r="G91" s="28"/>
       <c r="H91" s="13"/>
       <c r="I91" s="13"/>
       <c r="J91" s="5"/>
@@ -4323,7 +4410,7 @@
       <c r="D92" s="7"/>
       <c r="E92" s="12"/>
       <c r="F92" s="5"/>
-      <c r="G92" s="13"/>
+      <c r="G92" s="28"/>
       <c r="H92" s="13"/>
       <c r="I92" s="13"/>
       <c r="J92" s="5"/>
@@ -4343,7 +4430,7 @@
       <c r="D93" s="7"/>
       <c r="E93" s="12"/>
       <c r="F93" s="5"/>
-      <c r="G93" s="13"/>
+      <c r="G93" s="28"/>
       <c r="H93" s="13"/>
       <c r="I93" s="13"/>
       <c r="J93" s="5"/>
@@ -4363,7 +4450,7 @@
       <c r="D94" s="7"/>
       <c r="E94" s="12"/>
       <c r="F94" s="5"/>
-      <c r="G94" s="13"/>
+      <c r="G94" s="28"/>
       <c r="H94" s="13"/>
       <c r="I94" s="13"/>
       <c r="J94" s="5"/>
@@ -4383,7 +4470,7 @@
       <c r="D95" s="7"/>
       <c r="E95" s="12"/>
       <c r="F95" s="5"/>
-      <c r="G95" s="13"/>
+      <c r="G95" s="28"/>
       <c r="H95" s="13"/>
       <c r="I95" s="13"/>
       <c r="J95" s="5"/>
@@ -4403,7 +4490,7 @@
       <c r="D96" s="7"/>
       <c r="E96" s="12"/>
       <c r="F96" s="5"/>
-      <c r="G96" s="13"/>
+      <c r="G96" s="28"/>
       <c r="H96" s="13"/>
       <c r="I96" s="13"/>
       <c r="J96" s="5"/>
@@ -4423,7 +4510,7 @@
       <c r="D97" s="7"/>
       <c r="E97" s="12"/>
       <c r="F97" s="5"/>
-      <c r="G97" s="13"/>
+      <c r="G97" s="28"/>
       <c r="H97" s="13"/>
       <c r="I97" s="13"/>
       <c r="J97" s="5"/>
@@ -4443,7 +4530,7 @@
       <c r="D98" s="7"/>
       <c r="E98" s="12"/>
       <c r="F98" s="5"/>
-      <c r="G98" s="13"/>
+      <c r="G98" s="28"/>
       <c r="H98" s="13"/>
       <c r="I98" s="13"/>
       <c r="J98" s="5"/>
@@ -4463,7 +4550,7 @@
       <c r="D99" s="7"/>
       <c r="E99" s="12"/>
       <c r="F99" s="5"/>
-      <c r="G99" s="13"/>
+      <c r="G99" s="28"/>
       <c r="H99" s="13"/>
       <c r="I99" s="13"/>
       <c r="J99" s="5"/>
@@ -4483,7 +4570,7 @@
       <c r="D100" s="7"/>
       <c r="E100" s="12"/>
       <c r="F100" s="5"/>
-      <c r="G100" s="13"/>
+      <c r="G100" s="28"/>
       <c r="H100" s="13"/>
       <c r="I100" s="13"/>
       <c r="J100" s="5"/>
@@ -4503,7 +4590,7 @@
       <c r="D101" s="7"/>
       <c r="E101" s="12"/>
       <c r="F101" s="5"/>
-      <c r="G101" s="13"/>
+      <c r="G101" s="28"/>
       <c r="H101" s="13"/>
       <c r="I101" s="13"/>
       <c r="J101" s="5"/>
@@ -4523,7 +4610,7 @@
       <c r="D102" s="7"/>
       <c r="E102" s="12"/>
       <c r="F102" s="5"/>
-      <c r="G102" s="13"/>
+      <c r="G102" s="28"/>
       <c r="H102" s="13"/>
       <c r="I102" s="13"/>
       <c r="J102" s="5"/>
@@ -4543,7 +4630,7 @@
       <c r="D103" s="7"/>
       <c r="E103" s="12"/>
       <c r="F103" s="5"/>
-      <c r="G103" s="13"/>
+      <c r="G103" s="28"/>
       <c r="H103" s="13"/>
       <c r="I103" s="13"/>
       <c r="J103" s="5"/>
@@ -4563,7 +4650,7 @@
       <c r="D104" s="7"/>
       <c r="E104" s="12"/>
       <c r="F104" s="5"/>
-      <c r="G104" s="13"/>
+      <c r="G104" s="28"/>
       <c r="H104" s="13"/>
       <c r="I104" s="13"/>
       <c r="J104" s="5"/>
@@ -4583,7 +4670,7 @@
       <c r="D105" s="7"/>
       <c r="E105" s="12"/>
       <c r="F105" s="5"/>
-      <c r="G105" s="13"/>
+      <c r="G105" s="28"/>
       <c r="H105" s="13"/>
       <c r="I105" s="13"/>
       <c r="J105" s="5"/>
@@ -4603,7 +4690,7 @@
       <c r="D106" s="7"/>
       <c r="E106" s="12"/>
       <c r="F106" s="5"/>
-      <c r="G106" s="13"/>
+      <c r="G106" s="28"/>
       <c r="H106" s="13"/>
       <c r="I106" s="13"/>
       <c r="J106" s="5"/>
@@ -4623,7 +4710,7 @@
       <c r="D107" s="7"/>
       <c r="E107" s="12"/>
       <c r="F107" s="5"/>
-      <c r="G107" s="13"/>
+      <c r="G107" s="28"/>
       <c r="H107" s="13"/>
       <c r="I107" s="13"/>
       <c r="J107" s="5"/>
@@ -4643,7 +4730,7 @@
       <c r="D108" s="7"/>
       <c r="E108" s="12"/>
       <c r="F108" s="5"/>
-      <c r="G108" s="13"/>
+      <c r="G108" s="28"/>
       <c r="H108" s="13"/>
       <c r="I108" s="13"/>
       <c r="J108" s="5"/>
@@ -4663,7 +4750,7 @@
       <c r="D109" s="7"/>
       <c r="E109" s="12"/>
       <c r="F109" s="5"/>
-      <c r="G109" s="13"/>
+      <c r="G109" s="28"/>
       <c r="H109" s="13"/>
       <c r="I109" s="13"/>
       <c r="J109" s="5"/>
@@ -4683,7 +4770,7 @@
       <c r="D110" s="7"/>
       <c r="E110" s="12"/>
       <c r="F110" s="5"/>
-      <c r="G110" s="13"/>
+      <c r="G110" s="28"/>
       <c r="H110" s="13"/>
       <c r="I110" s="13"/>
       <c r="J110" s="5"/>
@@ -4703,7 +4790,7 @@
       <c r="D111" s="7"/>
       <c r="E111" s="12"/>
       <c r="F111" s="5"/>
-      <c r="G111" s="13"/>
+      <c r="G111" s="28"/>
       <c r="H111" s="13"/>
       <c r="I111" s="13"/>
       <c r="J111" s="5"/>
@@ -4723,7 +4810,7 @@
       <c r="D112" s="7"/>
       <c r="E112" s="12"/>
       <c r="F112" s="5"/>
-      <c r="G112" s="13"/>
+      <c r="G112" s="28"/>
       <c r="H112" s="13"/>
       <c r="I112" s="13"/>
       <c r="J112" s="5"/>
@@ -4743,7 +4830,7 @@
       <c r="D113" s="7"/>
       <c r="E113" s="12"/>
       <c r="F113" s="5"/>
-      <c r="G113" s="13"/>
+      <c r="G113" s="28"/>
       <c r="H113" s="13"/>
       <c r="I113" s="13"/>
       <c r="J113" s="5"/>
@@ -4763,7 +4850,7 @@
       <c r="D114" s="7"/>
       <c r="E114" s="12"/>
       <c r="F114" s="5"/>
-      <c r="G114" s="13"/>
+      <c r="G114" s="28"/>
       <c r="H114" s="13"/>
       <c r="I114" s="13"/>
       <c r="J114" s="5"/>
@@ -4772,9 +4859,6 @@
       <c r="M114" s="5"/>
       <c r="N114" s="13"/>
       <c r="O114" s="13"/>
-      <c r="P114" s="4" t="s">
-        <v>171</v>
-      </c>
     </row>
     <row r="115" spans="1:16" s="4" customFormat="1">
       <c r="A115" s="7"/>
@@ -4783,7 +4867,7 @@
       <c r="D115" s="7"/>
       <c r="E115" s="12"/>
       <c r="F115" s="5"/>
-      <c r="G115" s="13"/>
+      <c r="G115" s="28"/>
       <c r="H115" s="13"/>
       <c r="I115" s="13"/>
       <c r="J115" s="5"/>
@@ -4792,9 +4876,6 @@
       <c r="M115" s="5"/>
       <c r="N115" s="13"/>
       <c r="O115" s="13"/>
-      <c r="P115" s="4" t="s">
-        <v>172</v>
-      </c>
     </row>
     <row r="116" spans="1:16" s="4" customFormat="1">
       <c r="A116" s="7"/>
@@ -4803,7 +4884,7 @@
       <c r="D116" s="7"/>
       <c r="E116" s="12"/>
       <c r="F116" s="5"/>
-      <c r="G116" s="13"/>
+      <c r="G116" s="28"/>
       <c r="H116" s="13"/>
       <c r="I116" s="13"/>
       <c r="J116" s="5"/>
@@ -4812,9 +4893,6 @@
       <c r="M116" s="5"/>
       <c r="N116" s="13"/>
       <c r="O116" s="13"/>
-      <c r="P116" s="4" t="s">
-        <v>173</v>
-      </c>
     </row>
     <row r="117" spans="1:16" s="4" customFormat="1">
       <c r="A117" s="7"/>
@@ -4823,7 +4901,7 @@
       <c r="D117" s="7"/>
       <c r="E117" s="12"/>
       <c r="F117" s="5"/>
-      <c r="G117" s="13"/>
+      <c r="G117" s="28"/>
       <c r="H117" s="13"/>
       <c r="I117" s="13"/>
       <c r="J117" s="5"/>
@@ -4832,9 +4910,6 @@
       <c r="M117" s="5"/>
       <c r="N117" s="13"/>
       <c r="O117" s="13"/>
-      <c r="P117" s="4" t="s">
-        <v>174</v>
-      </c>
     </row>
     <row r="118" spans="1:16" s="4" customFormat="1">
       <c r="A118" s="7"/>
@@ -4843,7 +4918,7 @@
       <c r="D118" s="7"/>
       <c r="E118" s="12"/>
       <c r="F118" s="5"/>
-      <c r="G118" s="13"/>
+      <c r="G118" s="28"/>
       <c r="H118" s="13"/>
       <c r="I118" s="13"/>
       <c r="J118" s="5"/>
@@ -4852,9 +4927,6 @@
       <c r="M118" s="5"/>
       <c r="N118" s="13"/>
       <c r="O118" s="13"/>
-      <c r="P118" s="4" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="119" spans="1:16" s="4" customFormat="1">
       <c r="A119" s="7"/>
@@ -4863,7 +4935,7 @@
       <c r="D119" s="7"/>
       <c r="E119" s="12"/>
       <c r="F119" s="5"/>
-      <c r="G119" s="13"/>
+      <c r="G119" s="28"/>
       <c r="H119" s="13"/>
       <c r="I119" s="13"/>
       <c r="J119" s="5"/>
@@ -4872,9 +4944,6 @@
       <c r="M119" s="5"/>
       <c r="N119" s="13"/>
       <c r="O119" s="13"/>
-      <c r="P119" s="4" t="s">
-        <v>176</v>
-      </c>
     </row>
     <row r="120" spans="1:16" s="4" customFormat="1">
       <c r="A120" s="7"/>
@@ -4883,7 +4952,7 @@
       <c r="D120" s="7"/>
       <c r="E120" s="12"/>
       <c r="F120" s="5"/>
-      <c r="G120" s="13"/>
+      <c r="G120" s="28"/>
       <c r="H120" s="13"/>
       <c r="I120" s="13"/>
       <c r="J120" s="5"/>
@@ -4892,9 +4961,6 @@
       <c r="M120" s="5"/>
       <c r="N120" s="13"/>
       <c r="O120" s="13"/>
-      <c r="P120" s="4" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="121" spans="1:16" s="4" customFormat="1">
       <c r="A121" s="7"/>
@@ -4903,7 +4969,7 @@
       <c r="D121" s="7"/>
       <c r="E121" s="12"/>
       <c r="F121" s="5"/>
-      <c r="G121" s="13"/>
+      <c r="G121" s="28"/>
       <c r="H121" s="13"/>
       <c r="I121" s="13"/>
       <c r="J121" s="5"/>
@@ -4912,9 +4978,6 @@
       <c r="M121" s="5"/>
       <c r="N121" s="13"/>
       <c r="O121" s="13"/>
-      <c r="P121" s="4" t="s">
-        <v>178</v>
-      </c>
     </row>
     <row r="122" spans="1:16" s="4" customFormat="1">
       <c r="A122" s="7"/>
@@ -4923,7 +4986,7 @@
       <c r="D122" s="7"/>
       <c r="E122" s="12"/>
       <c r="F122" s="5"/>
-      <c r="G122" s="13"/>
+      <c r="G122" s="28"/>
       <c r="H122" s="13"/>
       <c r="I122" s="13"/>
       <c r="J122" s="5"/>
@@ -4932,9 +4995,6 @@
       <c r="M122" s="5"/>
       <c r="N122" s="13"/>
       <c r="O122" s="13"/>
-      <c r="P122" s="4" t="s">
-        <v>179</v>
-      </c>
     </row>
     <row r="123" spans="1:16" s="4" customFormat="1">
       <c r="A123" s="7"/>
@@ -4943,7 +5003,7 @@
       <c r="D123" s="7"/>
       <c r="E123" s="12"/>
       <c r="F123" s="5"/>
-      <c r="G123" s="13"/>
+      <c r="G123" s="28"/>
       <c r="H123" s="13"/>
       <c r="I123" s="13"/>
       <c r="J123" s="5"/>
@@ -4952,9 +5012,6 @@
       <c r="M123" s="5"/>
       <c r="N123" s="13"/>
       <c r="O123" s="13"/>
-      <c r="P123" s="4" t="s">
-        <v>180</v>
-      </c>
     </row>
     <row r="124" spans="1:16" s="4" customFormat="1">
       <c r="A124" s="7"/>
@@ -4963,7 +5020,7 @@
       <c r="D124" s="7"/>
       <c r="E124" s="12"/>
       <c r="F124" s="5"/>
-      <c r="G124" s="13"/>
+      <c r="G124" s="28"/>
       <c r="H124" s="13"/>
       <c r="I124" s="13"/>
       <c r="J124" s="5"/>
@@ -4972,9 +5029,6 @@
       <c r="M124" s="5"/>
       <c r="N124" s="13"/>
       <c r="O124" s="13"/>
-      <c r="P124" s="4" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="125" spans="1:16" s="4" customFormat="1">
       <c r="A125" s="7"/>
@@ -4983,7 +5037,7 @@
       <c r="D125" s="7"/>
       <c r="E125" s="12"/>
       <c r="F125" s="5"/>
-      <c r="G125" s="13"/>
+      <c r="G125" s="28"/>
       <c r="H125" s="13"/>
       <c r="I125" s="13"/>
       <c r="J125" s="5"/>
@@ -4992,9 +5046,6 @@
       <c r="M125" s="5"/>
       <c r="N125" s="13"/>
       <c r="O125" s="13"/>
-      <c r="P125" s="4" t="s">
-        <v>182</v>
-      </c>
     </row>
     <row r="126" spans="1:16" s="4" customFormat="1">
       <c r="A126" s="7"/>
@@ -5003,7 +5054,7 @@
       <c r="D126" s="7"/>
       <c r="E126" s="12"/>
       <c r="F126" s="5"/>
-      <c r="G126" s="13"/>
+      <c r="G126" s="28"/>
       <c r="H126" s="13"/>
       <c r="I126" s="13"/>
       <c r="J126" s="5"/>
@@ -5012,9 +5063,6 @@
       <c r="M126" s="5"/>
       <c r="N126" s="13"/>
       <c r="O126" s="13"/>
-      <c r="P126" s="4" t="s">
-        <v>183</v>
-      </c>
     </row>
     <row r="127" spans="1:16" s="4" customFormat="1">
       <c r="A127" s="7"/>
@@ -5023,7 +5071,7 @@
       <c r="D127" s="7"/>
       <c r="E127" s="12"/>
       <c r="F127" s="5"/>
-      <c r="G127" s="13"/>
+      <c r="G127" s="28"/>
       <c r="H127" s="13"/>
       <c r="I127" s="13"/>
       <c r="J127" s="5"/>
@@ -5032,9 +5080,6 @@
       <c r="M127" s="5"/>
       <c r="N127" s="13"/>
       <c r="O127" s="13"/>
-      <c r="P127" s="4" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="128" spans="1:16" s="4" customFormat="1">
       <c r="A128" s="7"/>
@@ -5043,7 +5088,7 @@
       <c r="D128" s="7"/>
       <c r="E128" s="12"/>
       <c r="F128" s="5"/>
-      <c r="G128" s="13"/>
+      <c r="G128" s="28"/>
       <c r="H128" s="13"/>
       <c r="I128" s="13"/>
       <c r="J128" s="5"/>
@@ -5060,7 +5105,7 @@
       <c r="D129" s="7"/>
       <c r="E129" s="12"/>
       <c r="F129" s="5"/>
-      <c r="G129" s="13"/>
+      <c r="G129" s="28"/>
       <c r="H129" s="13"/>
       <c r="I129" s="13"/>
       <c r="J129" s="5"/>
@@ -5077,7 +5122,7 @@
       <c r="D130" s="7"/>
       <c r="E130" s="12"/>
       <c r="F130" s="5"/>
-      <c r="G130" s="13"/>
+      <c r="G130" s="28"/>
       <c r="H130" s="13"/>
       <c r="I130" s="13"/>
       <c r="J130" s="5"/>
@@ -5094,7 +5139,7 @@
       <c r="D131" s="7"/>
       <c r="E131" s="12"/>
       <c r="F131" s="5"/>
-      <c r="G131" s="13"/>
+      <c r="G131" s="28"/>
       <c r="H131" s="13"/>
       <c r="I131" s="13"/>
       <c r="J131" s="5"/>
@@ -5111,7 +5156,7 @@
       <c r="D132" s="7"/>
       <c r="E132" s="12"/>
       <c r="F132" s="5"/>
-      <c r="G132" s="13"/>
+      <c r="G132" s="28"/>
       <c r="H132" s="13"/>
       <c r="I132" s="13"/>
       <c r="J132" s="5"/>
@@ -5128,7 +5173,7 @@
       <c r="D133" s="7"/>
       <c r="E133" s="12"/>
       <c r="F133" s="5"/>
-      <c r="G133" s="13"/>
+      <c r="G133" s="28"/>
       <c r="H133" s="13"/>
       <c r="I133" s="13"/>
       <c r="J133" s="5"/>
@@ -5145,7 +5190,7 @@
       <c r="D134" s="7"/>
       <c r="E134" s="12"/>
       <c r="F134" s="5"/>
-      <c r="G134" s="13"/>
+      <c r="G134" s="28"/>
       <c r="H134" s="13"/>
       <c r="I134" s="13"/>
       <c r="J134" s="5"/>
@@ -5162,7 +5207,7 @@
       <c r="D135" s="7"/>
       <c r="E135" s="12"/>
       <c r="F135" s="5"/>
-      <c r="G135" s="13"/>
+      <c r="G135" s="28"/>
       <c r="H135" s="13"/>
       <c r="I135" s="13"/>
       <c r="J135" s="5"/>
@@ -5179,7 +5224,7 @@
       <c r="D136" s="7"/>
       <c r="E136" s="12"/>
       <c r="F136" s="5"/>
-      <c r="G136" s="13"/>
+      <c r="G136" s="28"/>
       <c r="H136" s="13"/>
       <c r="I136" s="13"/>
       <c r="J136" s="5"/>
@@ -5196,7 +5241,7 @@
       <c r="D137" s="7"/>
       <c r="E137" s="12"/>
       <c r="F137" s="5"/>
-      <c r="G137" s="13"/>
+      <c r="G137" s="28"/>
       <c r="H137" s="13"/>
       <c r="I137" s="13"/>
       <c r="J137" s="5"/>
@@ -5213,7 +5258,7 @@
       <c r="D138" s="7"/>
       <c r="E138" s="12"/>
       <c r="F138" s="5"/>
-      <c r="G138" s="13"/>
+      <c r="G138" s="28"/>
       <c r="H138" s="13"/>
       <c r="I138" s="13"/>
       <c r="J138" s="5"/>
@@ -5230,7 +5275,7 @@
       <c r="D139" s="7"/>
       <c r="E139" s="12"/>
       <c r="F139" s="5"/>
-      <c r="G139" s="13"/>
+      <c r="G139" s="28"/>
       <c r="H139" s="13"/>
       <c r="I139" s="13"/>
       <c r="J139" s="5"/>
@@ -5247,7 +5292,7 @@
       <c r="D140" s="7"/>
       <c r="E140" s="12"/>
       <c r="F140" s="5"/>
-      <c r="G140" s="13"/>
+      <c r="G140" s="28"/>
       <c r="H140" s="13"/>
       <c r="I140" s="13"/>
       <c r="J140" s="5"/>
@@ -5264,7 +5309,7 @@
       <c r="D141" s="7"/>
       <c r="E141" s="12"/>
       <c r="F141" s="5"/>
-      <c r="G141" s="13"/>
+      <c r="G141" s="28"/>
       <c r="H141" s="13"/>
       <c r="I141" s="13"/>
       <c r="J141" s="5"/>
@@ -5281,7 +5326,7 @@
       <c r="D142" s="7"/>
       <c r="E142" s="12"/>
       <c r="F142" s="5"/>
-      <c r="G142" s="13"/>
+      <c r="G142" s="28"/>
       <c r="H142" s="13"/>
       <c r="I142" s="13"/>
       <c r="J142" s="5"/>
@@ -5298,7 +5343,7 @@
       <c r="D143" s="7"/>
       <c r="E143" s="12"/>
       <c r="F143" s="5"/>
-      <c r="G143" s="13"/>
+      <c r="G143" s="28"/>
       <c r="H143" s="13"/>
       <c r="I143" s="13"/>
       <c r="J143" s="5"/>
@@ -5315,7 +5360,7 @@
       <c r="D144" s="7"/>
       <c r="E144" s="12"/>
       <c r="F144" s="5"/>
-      <c r="G144" s="13"/>
+      <c r="G144" s="28"/>
       <c r="H144" s="13"/>
       <c r="I144" s="13"/>
       <c r="J144" s="5"/>
@@ -5332,7 +5377,7 @@
       <c r="D145" s="7"/>
       <c r="E145" s="12"/>
       <c r="F145" s="5"/>
-      <c r="G145" s="13"/>
+      <c r="G145" s="28"/>
       <c r="H145" s="13"/>
       <c r="I145" s="13"/>
       <c r="J145" s="5"/>
@@ -5349,7 +5394,7 @@
       <c r="D146" s="7"/>
       <c r="E146" s="12"/>
       <c r="F146" s="5"/>
-      <c r="G146" s="13"/>
+      <c r="G146" s="28"/>
       <c r="H146" s="13"/>
       <c r="I146" s="13"/>
       <c r="J146" s="5"/>
@@ -5366,7 +5411,7 @@
       <c r="D147" s="7"/>
       <c r="E147" s="12"/>
       <c r="F147" s="5"/>
-      <c r="G147" s="13"/>
+      <c r="G147" s="28"/>
       <c r="H147" s="13"/>
       <c r="I147" s="13"/>
       <c r="J147" s="5"/>
@@ -5383,7 +5428,7 @@
       <c r="D148" s="7"/>
       <c r="E148" s="12"/>
       <c r="F148" s="5"/>
-      <c r="G148" s="13"/>
+      <c r="G148" s="28"/>
       <c r="H148" s="13"/>
       <c r="I148" s="13"/>
       <c r="J148" s="5"/>
@@ -5400,7 +5445,7 @@
       <c r="D149" s="7"/>
       <c r="E149" s="12"/>
       <c r="F149" s="5"/>
-      <c r="G149" s="13"/>
+      <c r="G149" s="28"/>
       <c r="H149" s="13"/>
       <c r="I149" s="13"/>
       <c r="J149" s="5"/>
@@ -5417,7 +5462,7 @@
       <c r="D150" s="7"/>
       <c r="E150" s="12"/>
       <c r="F150" s="5"/>
-      <c r="G150" s="13"/>
+      <c r="G150" s="28"/>
       <c r="H150" s="13"/>
       <c r="I150" s="13"/>
       <c r="J150" s="5"/>
@@ -5434,7 +5479,7 @@
       <c r="D151" s="7"/>
       <c r="E151" s="12"/>
       <c r="F151" s="5"/>
-      <c r="G151" s="13"/>
+      <c r="G151" s="28"/>
       <c r="H151" s="13"/>
       <c r="I151" s="13"/>
       <c r="J151" s="5"/>
@@ -5451,7 +5496,7 @@
       <c r="D152" s="7"/>
       <c r="E152" s="12"/>
       <c r="F152" s="5"/>
-      <c r="G152" s="13"/>
+      <c r="G152" s="28"/>
       <c r="H152" s="13"/>
       <c r="I152" s="13"/>
       <c r="J152" s="5"/>
@@ -5468,7 +5513,7 @@
       <c r="D153" s="7"/>
       <c r="E153" s="12"/>
       <c r="F153" s="5"/>
-      <c r="G153" s="13"/>
+      <c r="G153" s="28"/>
       <c r="H153" s="13"/>
       <c r="I153" s="13"/>
       <c r="J153" s="5"/>
@@ -5485,7 +5530,7 @@
       <c r="D154" s="7"/>
       <c r="E154" s="12"/>
       <c r="F154" s="5"/>
-      <c r="G154" s="13"/>
+      <c r="G154" s="28"/>
       <c r="H154" s="13"/>
       <c r="I154" s="13"/>
       <c r="J154" s="5"/>
@@ -5502,7 +5547,7 @@
       <c r="D155" s="7"/>
       <c r="E155" s="12"/>
       <c r="F155" s="5"/>
-      <c r="G155" s="13"/>
+      <c r="G155" s="28"/>
       <c r="H155" s="13"/>
       <c r="I155" s="13"/>
       <c r="J155" s="5"/>
@@ -5519,7 +5564,7 @@
       <c r="D156" s="7"/>
       <c r="E156" s="12"/>
       <c r="F156" s="5"/>
-      <c r="G156" s="13"/>
+      <c r="G156" s="28"/>
       <c r="H156" s="13"/>
       <c r="I156" s="13"/>
       <c r="J156" s="5"/>
@@ -5536,7 +5581,7 @@
       <c r="D157" s="7"/>
       <c r="E157" s="12"/>
       <c r="F157" s="5"/>
-      <c r="G157" s="13"/>
+      <c r="G157" s="28"/>
       <c r="H157" s="13"/>
       <c r="I157" s="13"/>
       <c r="J157" s="5"/>
@@ -5553,7 +5598,7 @@
       <c r="D158" s="7"/>
       <c r="E158" s="12"/>
       <c r="F158" s="5"/>
-      <c r="G158" s="13"/>
+      <c r="G158" s="28"/>
       <c r="H158" s="13"/>
       <c r="I158" s="13"/>
       <c r="J158" s="5"/>
@@ -5570,7 +5615,7 @@
       <c r="D159" s="7"/>
       <c r="E159" s="12"/>
       <c r="F159" s="5"/>
-      <c r="G159" s="13"/>
+      <c r="G159" s="28"/>
       <c r="H159" s="13"/>
       <c r="I159" s="13"/>
       <c r="J159" s="5"/>
@@ -5587,7 +5632,7 @@
       <c r="D160" s="7"/>
       <c r="E160" s="12"/>
       <c r="F160" s="5"/>
-      <c r="G160" s="13"/>
+      <c r="G160" s="28"/>
       <c r="H160" s="13"/>
       <c r="I160" s="13"/>
       <c r="J160" s="5"/>
@@ -5604,7 +5649,7 @@
       <c r="D161" s="7"/>
       <c r="E161" s="12"/>
       <c r="F161" s="5"/>
-      <c r="G161" s="13"/>
+      <c r="G161" s="28"/>
       <c r="H161" s="13"/>
       <c r="I161" s="13"/>
       <c r="J161" s="5"/>
@@ -5621,7 +5666,7 @@
       <c r="D162" s="7"/>
       <c r="E162" s="12"/>
       <c r="F162" s="5"/>
-      <c r="G162" s="13"/>
+      <c r="G162" s="28"/>
       <c r="H162" s="13"/>
       <c r="I162" s="13"/>
       <c r="J162" s="5"/>
@@ -5638,7 +5683,7 @@
       <c r="D163" s="7"/>
       <c r="E163" s="12"/>
       <c r="F163" s="5"/>
-      <c r="G163" s="13"/>
+      <c r="G163" s="28"/>
       <c r="H163" s="13"/>
       <c r="I163" s="13"/>
       <c r="J163" s="5"/>
@@ -5655,7 +5700,7 @@
       <c r="D164" s="7"/>
       <c r="E164" s="12"/>
       <c r="F164" s="5"/>
-      <c r="G164" s="13"/>
+      <c r="G164" s="28"/>
       <c r="H164" s="13"/>
       <c r="I164" s="13"/>
       <c r="J164" s="5"/>
@@ -5672,7 +5717,7 @@
       <c r="D165" s="7"/>
       <c r="E165" s="12"/>
       <c r="F165" s="5"/>
-      <c r="G165" s="13"/>
+      <c r="G165" s="28"/>
       <c r="H165" s="13"/>
       <c r="I165" s="13"/>
       <c r="J165" s="5"/>
@@ -5689,7 +5734,7 @@
       <c r="D166" s="7"/>
       <c r="E166" s="12"/>
       <c r="F166" s="5"/>
-      <c r="G166" s="13"/>
+      <c r="G166" s="28"/>
       <c r="H166" s="13"/>
       <c r="I166" s="13"/>
       <c r="J166" s="5"/>
@@ -5706,7 +5751,7 @@
       <c r="D167" s="7"/>
       <c r="E167" s="12"/>
       <c r="F167" s="5"/>
-      <c r="G167" s="13"/>
+      <c r="G167" s="28"/>
       <c r="H167" s="13"/>
       <c r="I167" s="13"/>
       <c r="J167" s="5"/>
@@ -5723,7 +5768,7 @@
       <c r="D168" s="7"/>
       <c r="E168" s="12"/>
       <c r="F168" s="5"/>
-      <c r="G168" s="13"/>
+      <c r="G168" s="28"/>
       <c r="H168" s="13"/>
       <c r="I168" s="13"/>
       <c r="J168" s="5"/>
@@ -5740,7 +5785,7 @@
       <c r="D169" s="7"/>
       <c r="E169" s="12"/>
       <c r="F169" s="5"/>
-      <c r="G169" s="13"/>
+      <c r="G169" s="28"/>
       <c r="H169" s="13"/>
       <c r="I169" s="13"/>
       <c r="J169" s="5"/>
@@ -5757,7 +5802,7 @@
       <c r="D170" s="7"/>
       <c r="E170" s="12"/>
       <c r="F170" s="5"/>
-      <c r="G170" s="13"/>
+      <c r="G170" s="28"/>
       <c r="H170" s="13"/>
       <c r="I170" s="13"/>
       <c r="J170" s="5"/>
@@ -5774,7 +5819,7 @@
       <c r="D171" s="7"/>
       <c r="E171" s="12"/>
       <c r="F171" s="5"/>
-      <c r="G171" s="13"/>
+      <c r="G171" s="28"/>
       <c r="H171" s="13"/>
       <c r="I171" s="13"/>
       <c r="J171" s="5"/>
@@ -5791,7 +5836,7 @@
       <c r="D172" s="7"/>
       <c r="E172" s="12"/>
       <c r="F172" s="5"/>
-      <c r="G172" s="13"/>
+      <c r="G172" s="28"/>
       <c r="H172" s="13"/>
       <c r="I172" s="13"/>
       <c r="J172" s="5"/>
@@ -5808,7 +5853,7 @@
       <c r="D173" s="7"/>
       <c r="E173" s="12"/>
       <c r="F173" s="5"/>
-      <c r="G173" s="13"/>
+      <c r="G173" s="28"/>
       <c r="H173" s="13"/>
       <c r="I173" s="13"/>
       <c r="J173" s="5"/>
@@ -5825,7 +5870,7 @@
       <c r="D174" s="7"/>
       <c r="E174" s="12"/>
       <c r="F174" s="5"/>
-      <c r="G174" s="13"/>
+      <c r="G174" s="28"/>
       <c r="H174" s="13"/>
       <c r="I174" s="13"/>
       <c r="J174" s="5"/>
@@ -5842,7 +5887,7 @@
       <c r="D175" s="7"/>
       <c r="E175" s="12"/>
       <c r="F175" s="5"/>
-      <c r="G175" s="13"/>
+      <c r="G175" s="28"/>
       <c r="H175" s="13"/>
       <c r="I175" s="13"/>
       <c r="J175" s="5"/>
@@ -5859,7 +5904,7 @@
       <c r="D176" s="7"/>
       <c r="E176" s="12"/>
       <c r="F176" s="5"/>
-      <c r="G176" s="13"/>
+      <c r="G176" s="28"/>
       <c r="H176" s="13"/>
       <c r="I176" s="13"/>
       <c r="J176" s="5"/>
@@ -5876,7 +5921,7 @@
       <c r="D177" s="7"/>
       <c r="E177" s="12"/>
       <c r="F177" s="5"/>
-      <c r="G177" s="13"/>
+      <c r="G177" s="28"/>
       <c r="H177" s="13"/>
       <c r="I177" s="13"/>
       <c r="J177" s="5"/>
@@ -5893,7 +5938,7 @@
       <c r="D178" s="7"/>
       <c r="E178" s="12"/>
       <c r="F178" s="5"/>
-      <c r="G178" s="13"/>
+      <c r="G178" s="28"/>
       <c r="H178" s="13"/>
       <c r="I178" s="13"/>
       <c r="J178" s="5"/>
@@ -5910,7 +5955,7 @@
       <c r="D179" s="7"/>
       <c r="E179" s="12"/>
       <c r="F179" s="5"/>
-      <c r="G179" s="13"/>
+      <c r="G179" s="28"/>
       <c r="H179" s="13"/>
       <c r="I179" s="13"/>
       <c r="J179" s="5"/>
@@ -5927,7 +5972,7 @@
       <c r="D180" s="7"/>
       <c r="E180" s="12"/>
       <c r="F180" s="5"/>
-      <c r="G180" s="13"/>
+      <c r="G180" s="28"/>
       <c r="H180" s="13"/>
       <c r="I180" s="13"/>
       <c r="J180" s="5"/>
@@ -5944,7 +5989,7 @@
       <c r="D181" s="7"/>
       <c r="E181" s="12"/>
       <c r="F181" s="5"/>
-      <c r="G181" s="13"/>
+      <c r="G181" s="28"/>
       <c r="H181" s="13"/>
       <c r="I181" s="13"/>
       <c r="J181" s="5"/>
@@ -5961,7 +6006,7 @@
       <c r="D182" s="7"/>
       <c r="E182" s="12"/>
       <c r="F182" s="5"/>
-      <c r="G182" s="13"/>
+      <c r="G182" s="28"/>
       <c r="H182" s="13"/>
       <c r="I182" s="13"/>
       <c r="J182" s="5"/>
@@ -5978,7 +6023,7 @@
       <c r="D183" s="7"/>
       <c r="E183" s="12"/>
       <c r="F183" s="5"/>
-      <c r="G183" s="13"/>
+      <c r="G183" s="28"/>
       <c r="H183" s="13"/>
       <c r="I183" s="13"/>
       <c r="J183" s="5"/>
@@ -5995,7 +6040,7 @@
       <c r="D184" s="7"/>
       <c r="E184" s="12"/>
       <c r="F184" s="5"/>
-      <c r="G184" s="13"/>
+      <c r="G184" s="28"/>
       <c r="H184" s="13"/>
       <c r="I184" s="13"/>
       <c r="J184" s="5"/>
@@ -6012,7 +6057,7 @@
       <c r="D185" s="7"/>
       <c r="E185" s="12"/>
       <c r="F185" s="5"/>
-      <c r="G185" s="13"/>
+      <c r="G185" s="28"/>
       <c r="H185" s="13"/>
       <c r="I185" s="13"/>
       <c r="J185" s="5"/>
@@ -6029,7 +6074,7 @@
       <c r="D186" s="7"/>
       <c r="E186" s="12"/>
       <c r="F186" s="5"/>
-      <c r="G186" s="13"/>
+      <c r="G186" s="28"/>
       <c r="H186" s="13"/>
       <c r="I186" s="13"/>
       <c r="J186" s="5"/>
@@ -6046,7 +6091,7 @@
       <c r="D187" s="7"/>
       <c r="E187" s="12"/>
       <c r="F187" s="5"/>
-      <c r="G187" s="13"/>
+      <c r="G187" s="28"/>
       <c r="H187" s="13"/>
       <c r="I187" s="13"/>
       <c r="J187" s="5"/>
@@ -6063,7 +6108,7 @@
       <c r="D188" s="7"/>
       <c r="E188" s="12"/>
       <c r="F188" s="5"/>
-      <c r="G188" s="13"/>
+      <c r="G188" s="28"/>
       <c r="H188" s="13"/>
       <c r="I188" s="13"/>
       <c r="J188" s="5"/>
@@ -6080,7 +6125,7 @@
       <c r="D189" s="7"/>
       <c r="E189" s="12"/>
       <c r="F189" s="5"/>
-      <c r="G189" s="13"/>
+      <c r="G189" s="28"/>
       <c r="H189" s="13"/>
       <c r="I189" s="13"/>
       <c r="J189" s="5"/>
@@ -6097,7 +6142,7 @@
       <c r="D190" s="7"/>
       <c r="E190" s="12"/>
       <c r="F190" s="5"/>
-      <c r="G190" s="13"/>
+      <c r="G190" s="28"/>
       <c r="H190" s="13"/>
       <c r="I190" s="13"/>
       <c r="J190" s="5"/>
@@ -6114,7 +6159,7 @@
       <c r="D191" s="7"/>
       <c r="E191" s="12"/>
       <c r="F191" s="5"/>
-      <c r="G191" s="13"/>
+      <c r="G191" s="28"/>
       <c r="H191" s="13"/>
       <c r="I191" s="13"/>
       <c r="J191" s="5"/>
@@ -6131,7 +6176,7 @@
       <c r="D192" s="7"/>
       <c r="E192" s="12"/>
       <c r="F192" s="5"/>
-      <c r="G192" s="13"/>
+      <c r="G192" s="28"/>
       <c r="H192" s="13"/>
       <c r="I192" s="13"/>
       <c r="J192" s="5"/>
@@ -6148,7 +6193,7 @@
       <c r="D193" s="7"/>
       <c r="E193" s="12"/>
       <c r="F193" s="5"/>
-      <c r="G193" s="13"/>
+      <c r="G193" s="28"/>
       <c r="H193" s="13"/>
       <c r="I193" s="13"/>
       <c r="J193" s="5"/>
@@ -6165,7 +6210,7 @@
       <c r="D194" s="7"/>
       <c r="E194" s="12"/>
       <c r="F194" s="5"/>
-      <c r="G194" s="13"/>
+      <c r="G194" s="28"/>
       <c r="H194" s="13"/>
       <c r="I194" s="13"/>
       <c r="J194" s="5"/>
@@ -6182,7 +6227,7 @@
       <c r="D195" s="7"/>
       <c r="E195" s="12"/>
       <c r="F195" s="5"/>
-      <c r="G195" s="13"/>
+      <c r="G195" s="28"/>
       <c r="H195" s="13"/>
       <c r="I195" s="13"/>
       <c r="J195" s="5"/>
@@ -6199,7 +6244,7 @@
       <c r="D196" s="7"/>
       <c r="E196" s="12"/>
       <c r="F196" s="5"/>
-      <c r="G196" s="13"/>
+      <c r="G196" s="28"/>
       <c r="H196" s="13"/>
       <c r="I196" s="13"/>
       <c r="J196" s="5"/>
@@ -6216,7 +6261,7 @@
       <c r="D197" s="7"/>
       <c r="E197" s="12"/>
       <c r="F197" s="5"/>
-      <c r="G197" s="13"/>
+      <c r="G197" s="28"/>
       <c r="H197" s="13"/>
       <c r="I197" s="13"/>
       <c r="J197" s="5"/>
@@ -6233,7 +6278,7 @@
       <c r="D198" s="7"/>
       <c r="E198" s="12"/>
       <c r="F198" s="5"/>
-      <c r="G198" s="13"/>
+      <c r="G198" s="28"/>
       <c r="H198" s="13"/>
       <c r="I198" s="13"/>
       <c r="J198" s="5"/>
@@ -6250,7 +6295,7 @@
       <c r="D199" s="7"/>
       <c r="E199" s="12"/>
       <c r="F199" s="5"/>
-      <c r="G199" s="13"/>
+      <c r="G199" s="28"/>
       <c r="H199" s="13"/>
       <c r="I199" s="13"/>
       <c r="J199" s="5"/>
@@ -6267,7 +6312,7 @@
       <c r="D200" s="7"/>
       <c r="E200" s="12"/>
       <c r="F200" s="5"/>
-      <c r="G200" s="13"/>
+      <c r="G200" s="28"/>
       <c r="H200" s="13"/>
       <c r="I200" s="13"/>
       <c r="J200" s="5"/>
@@ -6284,7 +6329,7 @@
       <c r="D201" s="7"/>
       <c r="E201" s="12"/>
       <c r="F201" s="5"/>
-      <c r="G201" s="13"/>
+      <c r="G201" s="28"/>
       <c r="H201" s="13"/>
       <c r="I201" s="13"/>
       <c r="J201" s="5"/>
@@ -6301,7 +6346,7 @@
       <c r="D202" s="7"/>
       <c r="E202" s="12"/>
       <c r="F202" s="5"/>
-      <c r="G202" s="13"/>
+      <c r="G202" s="28"/>
       <c r="H202" s="13"/>
       <c r="I202" s="13"/>
       <c r="J202" s="5"/>
@@ -6318,7 +6363,7 @@
       <c r="D203" s="7"/>
       <c r="E203" s="12"/>
       <c r="F203" s="5"/>
-      <c r="G203" s="13"/>
+      <c r="G203" s="28"/>
       <c r="H203" s="13"/>
       <c r="I203" s="13"/>
       <c r="J203" s="5"/>
@@ -6335,7 +6380,7 @@
       <c r="D204" s="7"/>
       <c r="E204" s="12"/>
       <c r="F204" s="5"/>
-      <c r="G204" s="13"/>
+      <c r="G204" s="28"/>
       <c r="H204" s="13"/>
       <c r="I204" s="13"/>
       <c r="J204" s="5"/>
@@ -6352,7 +6397,7 @@
       <c r="D205" s="7"/>
       <c r="E205" s="12"/>
       <c r="F205" s="5"/>
-      <c r="G205" s="13"/>
+      <c r="G205" s="28"/>
       <c r="H205" s="13"/>
       <c r="I205" s="13"/>
       <c r="J205" s="5"/>
@@ -6369,7 +6414,7 @@
       <c r="D206" s="7"/>
       <c r="E206" s="12"/>
       <c r="F206" s="5"/>
-      <c r="G206" s="13"/>
+      <c r="G206" s="28"/>
       <c r="H206" s="13"/>
       <c r="I206" s="13"/>
       <c r="J206" s="5"/>
@@ -6386,7 +6431,7 @@
       <c r="D207" s="7"/>
       <c r="E207" s="12"/>
       <c r="F207" s="5"/>
-      <c r="G207" s="13"/>
+      <c r="G207" s="28"/>
       <c r="H207" s="13"/>
       <c r="I207" s="13"/>
       <c r="J207" s="5"/>
@@ -6403,7 +6448,7 @@
       <c r="D208" s="7"/>
       <c r="E208" s="12"/>
       <c r="F208" s="5"/>
-      <c r="G208" s="13"/>
+      <c r="G208" s="28"/>
       <c r="H208" s="13"/>
       <c r="I208" s="13"/>
       <c r="J208" s="5"/>
@@ -6420,7 +6465,7 @@
       <c r="D209" s="7"/>
       <c r="E209" s="12"/>
       <c r="F209" s="5"/>
-      <c r="G209" s="13"/>
+      <c r="G209" s="28"/>
       <c r="H209" s="13"/>
       <c r="I209" s="13"/>
       <c r="J209" s="5"/>
@@ -6437,7 +6482,7 @@
       <c r="D210" s="7"/>
       <c r="E210" s="12"/>
       <c r="F210" s="5"/>
-      <c r="G210" s="13"/>
+      <c r="G210" s="28"/>
       <c r="H210" s="13"/>
       <c r="I210" s="13"/>
       <c r="J210" s="5"/>
@@ -6454,7 +6499,7 @@
       <c r="D211" s="7"/>
       <c r="E211" s="12"/>
       <c r="F211" s="5"/>
-      <c r="G211" s="13"/>
+      <c r="G211" s="28"/>
       <c r="H211" s="13"/>
       <c r="I211" s="13"/>
       <c r="J211" s="5"/>
@@ -6471,7 +6516,7 @@
       <c r="D212" s="7"/>
       <c r="E212" s="12"/>
       <c r="F212" s="5"/>
-      <c r="G212" s="13"/>
+      <c r="G212" s="28"/>
       <c r="H212" s="13"/>
       <c r="I212" s="13"/>
       <c r="J212" s="5"/>
@@ -6488,7 +6533,7 @@
       <c r="D213" s="7"/>
       <c r="E213" s="12"/>
       <c r="F213" s="5"/>
-      <c r="G213" s="13"/>
+      <c r="G213" s="28"/>
       <c r="H213" s="13"/>
       <c r="I213" s="13"/>
       <c r="J213" s="5"/>
@@ -6505,7 +6550,7 @@
       <c r="D214" s="7"/>
       <c r="E214" s="12"/>
       <c r="F214" s="5"/>
-      <c r="G214" s="13"/>
+      <c r="G214" s="28"/>
       <c r="H214" s="13"/>
       <c r="I214" s="13"/>
       <c r="J214" s="5"/>
@@ -6522,7 +6567,7 @@
       <c r="D215" s="7"/>
       <c r="E215" s="12"/>
       <c r="F215" s="5"/>
-      <c r="G215" s="13"/>
+      <c r="G215" s="28"/>
       <c r="H215" s="13"/>
       <c r="I215" s="13"/>
       <c r="J215" s="5"/>
@@ -6539,7 +6584,7 @@
       <c r="D216" s="7"/>
       <c r="E216" s="12"/>
       <c r="F216" s="5"/>
-      <c r="G216" s="13"/>
+      <c r="G216" s="28"/>
       <c r="H216" s="13"/>
       <c r="I216" s="13"/>
       <c r="J216" s="5"/>
@@ -6556,7 +6601,7 @@
       <c r="D217" s="7"/>
       <c r="E217" s="12"/>
       <c r="F217" s="5"/>
-      <c r="G217" s="13"/>
+      <c r="G217" s="28"/>
       <c r="H217" s="13"/>
       <c r="I217" s="13"/>
       <c r="J217" s="5"/>
@@ -6573,7 +6618,7 @@
       <c r="D218" s="7"/>
       <c r="E218" s="12"/>
       <c r="F218" s="5"/>
-      <c r="G218" s="13"/>
+      <c r="G218" s="28"/>
       <c r="H218" s="13"/>
       <c r="I218" s="13"/>
       <c r="J218" s="5"/>
@@ -6590,7 +6635,7 @@
       <c r="D219" s="7"/>
       <c r="E219" s="12"/>
       <c r="F219" s="5"/>
-      <c r="G219" s="13"/>
+      <c r="G219" s="28"/>
       <c r="H219" s="13"/>
       <c r="I219" s="13"/>
       <c r="J219" s="5"/>
@@ -6607,7 +6652,7 @@
       <c r="D220" s="7"/>
       <c r="E220" s="12"/>
       <c r="F220" s="5"/>
-      <c r="G220" s="13"/>
+      <c r="G220" s="28"/>
       <c r="H220" s="13"/>
       <c r="I220" s="13"/>
       <c r="J220" s="5"/>
@@ -6617,251 +6662,13 @@
       <c r="N220" s="13"/>
       <c r="O220" s="13"/>
     </row>
-    <row r="221" spans="1:15" s="4" customFormat="1">
-      <c r="A221" s="7"/>
-      <c r="B221" s="7"/>
-      <c r="C221" s="5"/>
-      <c r="D221" s="7"/>
-      <c r="E221" s="12"/>
-      <c r="F221" s="5"/>
-      <c r="G221" s="13"/>
-      <c r="H221" s="13"/>
-      <c r="I221" s="13"/>
-      <c r="J221" s="5"/>
-      <c r="K221" s="5"/>
-      <c r="L221" s="5"/>
-      <c r="M221" s="5"/>
-      <c r="N221" s="13"/>
-      <c r="O221" s="13"/>
-    </row>
-    <row r="222" spans="1:15" s="4" customFormat="1">
-      <c r="A222" s="7"/>
-      <c r="B222" s="7"/>
-      <c r="C222" s="5"/>
-      <c r="D222" s="7"/>
-      <c r="E222" s="12"/>
-      <c r="F222" s="5"/>
-      <c r="G222" s="13"/>
-      <c r="H222" s="13"/>
-      <c r="I222" s="13"/>
-      <c r="J222" s="5"/>
-      <c r="K222" s="5"/>
-      <c r="L222" s="5"/>
-      <c r="M222" s="5"/>
-      <c r="N222" s="13"/>
-      <c r="O222" s="13"/>
-    </row>
-    <row r="223" spans="1:15" s="4" customFormat="1">
-      <c r="A223" s="7"/>
-      <c r="B223" s="7"/>
-      <c r="C223" s="5"/>
-      <c r="D223" s="7"/>
-      <c r="E223" s="12"/>
-      <c r="F223" s="5"/>
-      <c r="G223" s="13"/>
-      <c r="H223" s="13"/>
-      <c r="I223" s="13"/>
-      <c r="J223" s="5"/>
-      <c r="K223" s="5"/>
-      <c r="L223" s="5"/>
-      <c r="M223" s="5"/>
-      <c r="N223" s="13"/>
-      <c r="O223" s="13"/>
-    </row>
-    <row r="224" spans="1:15" s="4" customFormat="1">
-      <c r="A224" s="7"/>
-      <c r="B224" s="7"/>
-      <c r="C224" s="5"/>
-      <c r="D224" s="7"/>
-      <c r="E224" s="12"/>
-      <c r="F224" s="5"/>
-      <c r="G224" s="13"/>
-      <c r="H224" s="13"/>
-      <c r="I224" s="13"/>
-      <c r="J224" s="5"/>
-      <c r="K224" s="5"/>
-      <c r="L224" s="5"/>
-      <c r="M224" s="5"/>
-      <c r="N224" s="13"/>
-      <c r="O224" s="13"/>
-    </row>
-    <row r="225" spans="1:15" s="4" customFormat="1">
-      <c r="A225" s="7"/>
-      <c r="B225" s="7"/>
-      <c r="C225" s="5"/>
-      <c r="D225" s="7"/>
-      <c r="E225" s="12"/>
-      <c r="F225" s="5"/>
-      <c r="G225" s="13"/>
-      <c r="H225" s="13"/>
-      <c r="I225" s="13"/>
-      <c r="J225" s="5"/>
-      <c r="K225" s="5"/>
-      <c r="L225" s="5"/>
-      <c r="M225" s="5"/>
-      <c r="N225" s="13"/>
-      <c r="O225" s="13"/>
-    </row>
-    <row r="226" spans="1:15" s="4" customFormat="1">
-      <c r="A226" s="7"/>
-      <c r="B226" s="7"/>
-      <c r="C226" s="5"/>
-      <c r="D226" s="7"/>
-      <c r="E226" s="12"/>
-      <c r="F226" s="5"/>
-      <c r="G226" s="13"/>
-      <c r="H226" s="13"/>
-      <c r="I226" s="13"/>
-      <c r="J226" s="5"/>
-      <c r="K226" s="5"/>
-      <c r="L226" s="5"/>
-      <c r="M226" s="5"/>
-      <c r="N226" s="13"/>
-      <c r="O226" s="13"/>
-    </row>
-    <row r="227" spans="1:15" s="4" customFormat="1">
-      <c r="A227" s="7"/>
-      <c r="B227" s="7"/>
-      <c r="C227" s="5"/>
-      <c r="D227" s="7"/>
-      <c r="E227" s="12"/>
-      <c r="F227" s="5"/>
-      <c r="G227" s="13"/>
-      <c r="H227" s="13"/>
-      <c r="I227" s="13"/>
-      <c r="J227" s="5"/>
-      <c r="K227" s="5"/>
-      <c r="L227" s="5"/>
-      <c r="M227" s="5"/>
-      <c r="N227" s="13"/>
-      <c r="O227" s="13"/>
-    </row>
-    <row r="228" spans="1:15" s="4" customFormat="1">
-      <c r="A228" s="7"/>
-      <c r="B228" s="7"/>
-      <c r="C228" s="5"/>
-      <c r="D228" s="7"/>
-      <c r="E228" s="12"/>
-      <c r="F228" s="5"/>
-      <c r="G228" s="13"/>
-      <c r="H228" s="13"/>
-      <c r="I228" s="13"/>
-      <c r="J228" s="5"/>
-      <c r="K228" s="5"/>
-      <c r="L228" s="5"/>
-      <c r="M228" s="5"/>
-      <c r="N228" s="13"/>
-      <c r="O228" s="13"/>
-    </row>
-    <row r="229" spans="1:15" s="4" customFormat="1">
-      <c r="A229" s="7"/>
-      <c r="B229" s="7"/>
-      <c r="C229" s="5"/>
-      <c r="D229" s="7"/>
-      <c r="E229" s="12"/>
-      <c r="F229" s="5"/>
-      <c r="G229" s="13"/>
-      <c r="H229" s="13"/>
-      <c r="I229" s="13"/>
-      <c r="J229" s="5"/>
-      <c r="K229" s="5"/>
-      <c r="L229" s="5"/>
-      <c r="M229" s="5"/>
-      <c r="N229" s="13"/>
-      <c r="O229" s="13"/>
-    </row>
-    <row r="230" spans="1:15" s="4" customFormat="1">
-      <c r="A230" s="7"/>
-      <c r="B230" s="7"/>
-      <c r="C230" s="5"/>
-      <c r="D230" s="7"/>
-      <c r="E230" s="12"/>
-      <c r="F230" s="5"/>
-      <c r="G230" s="13"/>
-      <c r="H230" s="13"/>
-      <c r="I230" s="13"/>
-      <c r="J230" s="5"/>
-      <c r="K230" s="5"/>
-      <c r="L230" s="5"/>
-      <c r="M230" s="5"/>
-      <c r="N230" s="13"/>
-      <c r="O230" s="13"/>
-    </row>
-    <row r="231" spans="1:15" s="4" customFormat="1">
-      <c r="A231" s="7"/>
-      <c r="B231" s="7"/>
-      <c r="C231" s="5"/>
-      <c r="D231" s="7"/>
-      <c r="E231" s="12"/>
-      <c r="F231" s="5"/>
-      <c r="G231" s="13"/>
-      <c r="H231" s="13"/>
-      <c r="I231" s="13"/>
-      <c r="J231" s="5"/>
-      <c r="K231" s="5"/>
-      <c r="L231" s="5"/>
-      <c r="M231" s="5"/>
-      <c r="N231" s="13"/>
-      <c r="O231" s="13"/>
-    </row>
-    <row r="232" spans="1:15" s="4" customFormat="1">
-      <c r="A232" s="7"/>
-      <c r="B232" s="7"/>
-      <c r="C232" s="5"/>
-      <c r="D232" s="7"/>
-      <c r="E232" s="12"/>
-      <c r="F232" s="5"/>
-      <c r="G232" s="13"/>
-      <c r="H232" s="13"/>
-      <c r="I232" s="13"/>
-      <c r="J232" s="5"/>
-      <c r="K232" s="5"/>
-      <c r="L232" s="5"/>
-      <c r="M232" s="5"/>
-      <c r="N232" s="13"/>
-      <c r="O232" s="13"/>
-    </row>
-    <row r="233" spans="1:15" s="4" customFormat="1">
-      <c r="A233" s="7"/>
-      <c r="B233" s="7"/>
-      <c r="C233" s="5"/>
-      <c r="D233" s="7"/>
-      <c r="E233" s="12"/>
-      <c r="F233" s="5"/>
-      <c r="G233" s="13"/>
-      <c r="H233" s="13"/>
-      <c r="I233" s="13"/>
-      <c r="J233" s="5"/>
-      <c r="K233" s="5"/>
-      <c r="L233" s="5"/>
-      <c r="M233" s="5"/>
-      <c r="N233" s="13"/>
-      <c r="O233" s="13"/>
-    </row>
-    <row r="234" spans="1:15" s="4" customFormat="1">
-      <c r="A234" s="7"/>
-      <c r="B234" s="7"/>
-      <c r="C234" s="5"/>
-      <c r="D234" s="7"/>
-      <c r="E234" s="12"/>
-      <c r="F234" s="5"/>
-      <c r="G234" s="13"/>
-      <c r="H234" s="13"/>
-      <c r="I234" s="13"/>
-      <c r="J234" s="5"/>
-      <c r="K234" s="5"/>
-      <c r="L234" s="5"/>
-      <c r="M234" s="5"/>
-      <c r="N234" s="13"/>
-      <c r="O234" s="13"/>
-    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" sqref="F8:F234">
+    <dataValidation type="list" sqref="F13:F220">
       <formula1>P$1:P$7</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="E2:E7">
-      <formula1>O$1:O$133</formula1>
+    <dataValidation type="list" sqref="E2:E12">
+      <formula1>O$1:O$119</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>